<commit_message>
Some stuff - want a branch for as a sand box
</commit_message>
<xml_diff>
--- a/Applications/StatsAppFunctionality_MOSCOW.xlsx
+++ b/Applications/StatsAppFunctionality_MOSCOW.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="122">
   <si>
     <t>functionality for the statsapp:</t>
   </si>
@@ -255,13 +255,148 @@
   </si>
   <si>
     <t>Visual data and graphs</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application to generate and populate the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">database with a large number of </t>
+  </si>
+  <si>
+    <t>random 4-char codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application for visitor support in cases </t>
+  </si>
+  <si>
+    <t>of identification-related exceptions and other</t>
+  </si>
+  <si>
+    <t>issues</t>
+  </si>
+  <si>
+    <t>Notification Center</t>
+  </si>
+  <si>
+    <t>Application for the shops and sale points</t>
+  </si>
+  <si>
+    <t>Paused due to issues</t>
+  </si>
+  <si>
+    <t>General APP</t>
+  </si>
+  <si>
+    <t>Application for assigning and deactivating bracelets</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Requires modifications in logics behind assigning new</t>
+  </si>
+  <si>
+    <t>bracelets</t>
+  </si>
+  <si>
+    <t>Application for controlling the event entrance procedure</t>
+  </si>
+  <si>
+    <t>Application for entering the reserved activity</t>
+  </si>
+  <si>
+    <t>Stable - Frozen</t>
+  </si>
+  <si>
+    <t>Stable - Testing stage</t>
+  </si>
+  <si>
+    <t>Application for generating random codes</t>
+  </si>
+  <si>
+    <t>Administrative application for data tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application for controlling the camping </t>
+  </si>
+  <si>
+    <t>entrance procedure</t>
+  </si>
+  <si>
+    <t>Application for the tent payment terminal</t>
+  </si>
+  <si>
+    <t>and inspecting the status of the event</t>
+  </si>
+  <si>
+    <t>Application for loaning the necessary equipment</t>
+  </si>
+  <si>
+    <t>Considered {Only extras left}</t>
+  </si>
+  <si>
+    <t>Application for entering the activity entrance</t>
+  </si>
+  <si>
+    <t>new tables for archives</t>
+  </si>
+  <si>
+    <t>a lot of views</t>
+  </si>
+  <si>
+    <t>scheduled events to generate t.data</t>
+  </si>
+  <si>
+    <t>General app functionality:</t>
+  </si>
+  <si>
+    <t>Starting other applications</t>
+  </si>
+  <si>
+    <t>Sending data</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>Employee complaints and notificiations</t>
+  </si>
+  <si>
+    <t>Alerts and alarms</t>
+  </si>
+  <si>
+    <t>User verification</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>General statistical information</t>
+  </si>
+  <si>
+    <t>Loaning app functionality:</t>
+  </si>
+  <si>
+    <t>Barcode scanner</t>
+  </si>
+  <si>
+    <t>Registring returns and issues of the items</t>
+  </si>
+  <si>
+    <t>Adding new items to the database</t>
+  </si>
+  <si>
+    <t>If missed the due data ask to pay more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the missed payment alert to a respective db </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +442,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +511,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -398,13 +582,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -428,10 +614,17 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
@@ -713,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1303,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>19</v>
       </c>
@@ -1123,7 +1316,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>22</v>
       </c>
@@ -1136,7 +1329,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>23</v>
       </c>
@@ -1149,7 +1342,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
@@ -1161,8 +1354,44 @@
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
       <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE20" s="27"/>
+      <c r="AF20" s="27"/>
+      <c r="AG20" s="27"/>
+      <c r="AH20" s="27"/>
+      <c r="AI20" s="27"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>25</v>
       </c>
@@ -1174,8 +1403,23 @@
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O21" t="s">
+        <v>97</v>
+      </c>
+      <c r="T21" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>40</v>
       </c>
@@ -1187,8 +1431,17 @@
         <v>20</v>
       </c>
       <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>39</v>
       </c>
@@ -1200,8 +1453,14 @@
         <v>20</v>
       </c>
       <c r="G23" s="20"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>38</v>
       </c>
@@ -1213,8 +1472,11 @@
         <v>20</v>
       </c>
       <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>57</v>
       </c>
@@ -1226,35 +1488,68 @@
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="J25" t="s">
+        <v>81</v>
+      </c>
+      <c r="O25" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>104</v>
+      </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
+      <c r="D26" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
       <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="J26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="F27" s="19"/>
       <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="J27" t="s">
+        <v>83</v>
+      </c>
+      <c r="O27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
+      <c r="D28" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1262,8 +1557,14 @@
       <c r="E29" s="18"/>
       <c r="F29" s="19"/>
       <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>84</v>
+      </c>
+      <c r="O29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1272,7 +1573,7 @@
       <c r="F30" s="19"/>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1280,8 +1581,14 @@
       <c r="E31" s="18"/>
       <c r="F31" s="19"/>
       <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>95</v>
+      </c>
+      <c r="O31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1290,7 +1597,7 @@
       <c r="F32" s="19"/>
       <c r="G32" s="20"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1299,7 +1606,7 @@
       <c r="F33" s="19"/>
       <c r="G33" s="20"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1308,7 +1615,7 @@
       <c r="F34" s="19"/>
       <c r="G34" s="20"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1317,7 +1624,7 @@
       <c r="F35" s="19"/>
       <c r="G35" s="20"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1326,7 +1633,7 @@
       <c r="F36" s="19"/>
       <c r="G36" s="20"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1335,7 +1642,7 @@
       <c r="F37" s="19"/>
       <c r="G37" s="20"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1343,8 +1650,22 @@
       <c r="E38" s="18"/>
       <c r="F38" s="19"/>
       <c r="G38" s="20"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1352,8 +1673,14 @@
       <c r="E39" s="18"/>
       <c r="F39" s="19"/>
       <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>108</v>
+      </c>
+      <c r="O39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1361,8 +1688,14 @@
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
       <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>109</v>
+      </c>
+      <c r="O40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1370,8 +1703,14 @@
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
       <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>110</v>
+      </c>
+      <c r="O41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1379,8 +1718,14 @@
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
       <c r="G42" s="20"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>111</v>
+      </c>
+      <c r="O42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1388,8 +1733,14 @@
       <c r="E43" s="18"/>
       <c r="F43" s="19"/>
       <c r="G43" s="20"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>112</v>
+      </c>
+      <c r="O43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1397,8 +1748,11 @@
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
       <c r="G44" s="20"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1406,8 +1760,11 @@
       <c r="E45" s="18"/>
       <c r="F45" s="19"/>
       <c r="G45" s="20"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -1415,8 +1772,11 @@
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
       <c r="G46" s="20"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -1425,7 +1785,7 @@
       <c r="F47" s="19"/>
       <c r="G47" s="20"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>

</xml_diff>